<commit_message>
Improved scripts for estimating Budapest potentials
</commit_message>
<xml_diff>
--- a/results_v9_with_groundwater_flow.xlsx
+++ b/results_v9_with_groundwater_flow.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,785 +434,1091 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Geology</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Geology</t>
+          <t>L_borehole</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>L_borehole</t>
+          <t>borehole_spacing</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>borehole_spacing</t>
+          <t>E_annual</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>E_annual</t>
+          <t>R_squared</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>R_squared</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>RMSE</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>B-21</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>9.21844983876221</v>
       </c>
       <c r="E2" t="n">
-        <v>9.21844983876221</v>
+        <v>0.9999040167983522</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9999040167983522</v>
-      </c>
-      <c r="G2" t="n">
         <v>0.1090164142884328</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>B-30</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>100</v>
+      </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>9.17497265829096</v>
       </c>
       <c r="E3" t="n">
-        <v>9.17497265829096</v>
+        <v>0.9999037437796786</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9999037437796786</v>
-      </c>
-      <c r="G3" t="n">
         <v>0.108854500070686</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>B-39</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>7.850345155974851</v>
       </c>
       <c r="E4" t="n">
-        <v>7.850345155974851</v>
+        <v>0.9998679555139213</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9998679555139213</v>
-      </c>
-      <c r="G4" t="n">
         <v>0.1496853065093049</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>B-48</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>7.122845123382458</v>
       </c>
       <c r="E5" t="n">
-        <v>7.122845123382458</v>
+        <v>0.9998868613193341</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9998868613193341</v>
-      </c>
-      <c r="G5" t="n">
         <v>0.1505500700776748</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>B-63</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
       <c r="C6" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>7.467579227324548</v>
       </c>
       <c r="E6" t="n">
-        <v>7.467579227324548</v>
+        <v>0.9998543253607863</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9998543253607863</v>
-      </c>
-      <c r="G6" t="n">
         <v>0.1630397871234354</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>B-13</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>7.146325243609454</v>
       </c>
       <c r="E7" t="n">
-        <v>7.146325243609454</v>
+        <v>0.9998866809397818</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9998866809397818</v>
-      </c>
-      <c r="G7" t="n">
         <v>0.1488489961636213</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>B-56</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>7.191361310805442</v>
       </c>
       <c r="E8" t="n">
-        <v>7.191361310805442</v>
+        <v>0.9998538776625517</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9998538776625517</v>
-      </c>
-      <c r="G8" t="n">
         <v>0.1682874050657907</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>B-179</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
       <c r="C9" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>20</v>
+        <v>6.945796764116369</v>
       </c>
       <c r="E9" t="n">
-        <v>6.945796764116369</v>
+        <v>0.9998536857540545</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9998536857540545</v>
-      </c>
-      <c r="G9" t="n">
         <v>0.1763541527660759</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>B-180</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>100</v>
+      </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>6.944631728693515</v>
       </c>
       <c r="E10" t="n">
-        <v>6.944631728693515</v>
+        <v>0.9998538951148055</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9998538951148055</v>
-      </c>
-      <c r="G10" t="n">
         <v>0.1762140130145536</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Pm_1</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>100</v>
+      </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>6.965091855721885</v>
       </c>
       <c r="E11" t="n">
-        <v>6.965091855721885</v>
+        <v>0.9998865828366261</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9998865828366261</v>
-      </c>
-      <c r="G11" t="n">
         <v>0.1497434259320005</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>B-64</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>20</v>
+        <v>7.262139760740293</v>
       </c>
       <c r="E12" t="n">
-        <v>7.262139760740293</v>
+        <v>0.9998866047383963</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9998866047383963</v>
-      </c>
-      <c r="G12" t="n">
         <v>0.1482866879111396</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>B-38</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>100</v>
+      </c>
       <c r="C13" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>20</v>
+        <v>9.436236075871955</v>
       </c>
       <c r="E13" t="n">
-        <v>9.436236075871955</v>
+        <v>0.9999663379257652</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9999663379257652</v>
-      </c>
-      <c r="G13" t="n">
         <v>0.06296544555103455</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>B-21</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>100</v>
+      </c>
       <c r="C14" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>500</v>
+        <v>13.80309012381412</v>
       </c>
       <c r="E14" t="n">
-        <v>13.80309012381412</v>
+        <v>0.9999755569529967</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9999755569529967</v>
-      </c>
-      <c r="G14" t="n">
         <v>0.03621290221125383</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>B-30</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>100</v>
+      </c>
       <c r="C15" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D15" t="n">
-        <v>500</v>
+        <v>13.75349855115748</v>
       </c>
       <c r="E15" t="n">
-        <v>13.75349855115748</v>
+        <v>0.9999755822586712</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9999755822586712</v>
-      </c>
-      <c r="G15" t="n">
         <v>0.03604427696486062</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>B-39</t>
         </is>
       </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
       <c r="C16" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D16" t="n">
-        <v>500</v>
+        <v>14.71828898885477</v>
       </c>
       <c r="E16" t="n">
-        <v>14.71828898885477</v>
+        <v>0.9999999999997828</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9999999999997828</v>
-      </c>
-      <c r="G16" t="n">
         <v>3.142121239035844e-06</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>B-48</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
       <c r="C17" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D17" t="n">
-        <v>500</v>
+        <v>13.93039025553758</v>
       </c>
       <c r="E17" t="n">
-        <v>13.93039025553758</v>
+        <v>0.9999629326952517</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9999629326952517</v>
-      </c>
-      <c r="G17" t="n">
         <v>0.04311266679580261</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>B-63</t>
         </is>
       </c>
+      <c r="B18" t="n">
+        <v>100</v>
+      </c>
       <c r="C18" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D18" t="n">
-        <v>500</v>
+        <v>14.65735520684417</v>
       </c>
       <c r="E18" t="n">
-        <v>14.65735520684417</v>
+        <v>0.9999810066005708</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9999810066005708</v>
-      </c>
-      <c r="G18" t="n">
         <v>0.02918720305466918</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>B-13</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>100</v>
+      </c>
       <c r="C19" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D19" t="n">
-        <v>500</v>
+        <v>14.09122038923292</v>
       </c>
       <c r="E19" t="n">
-        <v>14.09122038923292</v>
+        <v>0.9999999999996614</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9999999999996614</v>
-      </c>
-      <c r="G19" t="n">
         <v>4.002304269794799e-06</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>B-56</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>100</v>
+      </c>
       <c r="C20" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D20" t="n">
-        <v>500</v>
+        <v>14.03593554125328</v>
       </c>
       <c r="E20" t="n">
-        <v>14.03593554125328</v>
+        <v>0.999954137153104</v>
       </c>
       <c r="F20" t="n">
-        <v>0.999954137153104</v>
-      </c>
-      <c r="G20" t="n">
         <v>0.04712186651722308</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>B-179</t>
         </is>
       </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
       <c r="C21" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D21" t="n">
-        <v>500</v>
+        <v>13.7641126814821</v>
       </c>
       <c r="E21" t="n">
-        <v>13.7641126814821</v>
+        <v>0.9999999999988514</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9999999999988514</v>
-      </c>
-      <c r="G21" t="n">
         <v>7.607552932735919e-06</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>B-180</t>
         </is>
       </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
       <c r="C22" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D22" t="n">
-        <v>500</v>
+        <v>13.75785640790028</v>
       </c>
       <c r="E22" t="n">
-        <v>13.75785640790028</v>
+        <v>0.9999999999994116</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9999999999994116</v>
-      </c>
-      <c r="G22" t="n">
         <v>5.446096517442401e-06</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Pm_1</t>
         </is>
       </c>
+      <c r="B23" t="n">
+        <v>100</v>
+      </c>
       <c r="C23" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D23" t="n">
-        <v>500</v>
+        <v>13.72587843934187</v>
       </c>
       <c r="E23" t="n">
-        <v>13.72587843934187</v>
+        <v>0.9999999999997945</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9999999999997945</v>
-      </c>
-      <c r="G23" t="n">
         <v>3.135255900472722e-06</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>B-64</t>
         </is>
       </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
       <c r="C24" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D24" t="n">
-        <v>500</v>
+        <v>14.21619012860485</v>
       </c>
       <c r="E24" t="n">
-        <v>14.21619012860485</v>
+        <v>0.9999472454199009</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9999472454199009</v>
-      </c>
-      <c r="G24" t="n">
         <v>0.05065950956896099</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>B-38</t>
         </is>
       </c>
+      <c r="B25" t="n">
+        <v>100</v>
+      </c>
       <c r="C25" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D25" t="n">
-        <v>500</v>
+        <v>14.29902609073449</v>
       </c>
       <c r="E25" t="n">
-        <v>14.29902609073449</v>
+        <v>0.9999999999878484</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9999999999878484</v>
-      </c>
-      <c r="G25" t="n">
         <v>2.465577087570636e-05</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>B-21</t>
         </is>
       </c>
+      <c r="B26" t="n">
+        <v>200</v>
+      </c>
       <c r="C26" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>20</v>
+        <v>20.0842665752264</v>
       </c>
       <c r="E26" t="n">
-        <v>20.0842665752264</v>
+        <v>0.999999999998341</v>
       </c>
       <c r="F26" t="n">
-        <v>0.999999999998341</v>
-      </c>
-      <c r="G26" t="n">
         <v>7.720521867532577e-06</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>B-30</t>
         </is>
       </c>
+      <c r="B27" t="n">
+        <v>200</v>
+      </c>
       <c r="C27" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D27" t="n">
-        <v>20</v>
+        <v>19.86126465990586</v>
       </c>
       <c r="E27" t="n">
-        <v>19.86126465990586</v>
+        <v>0.9999999999977286</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9999999999977286</v>
-      </c>
-      <c r="G27" t="n">
         <v>9.021711163518374e-06</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>B-39</t>
         </is>
       </c>
+      <c r="B28" t="n">
+        <v>200</v>
+      </c>
       <c r="C28" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>20</v>
+        <v>15.66255510631849</v>
       </c>
       <c r="E28" t="n">
-        <v>15.66255510631849</v>
+        <v>0.9999999998934743</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9999999998934743</v>
-      </c>
-      <c r="G28" t="n">
         <v>7.734172792830801e-05</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>B-48</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>200</v>
+      </c>
       <c r="C29" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
+        <v>13.74003643341299</v>
       </c>
       <c r="E29" t="n">
-        <v>13.74003643341299</v>
+        <v>0.9999999999326177</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9999999999326177</v>
-      </c>
-      <c r="G29" t="n">
         <v>6.801460274817656e-05</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>B-63</t>
         </is>
       </c>
+      <c r="B30" t="n">
+        <v>200</v>
+      </c>
       <c r="C30" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D30" t="n">
-        <v>20</v>
+        <v>14.14044927242644</v>
       </c>
       <c r="E30" t="n">
-        <v>14.14044927242644</v>
+        <v>0.9999999999998527</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9999999999998527</v>
-      </c>
-      <c r="G30" t="n">
         <v>3.112600387289358e-06</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>B-13</t>
         </is>
       </c>
+      <c r="B31" t="n">
+        <v>200</v>
+      </c>
       <c r="C31" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>13.6350407326293</v>
       </c>
       <c r="E31" t="n">
-        <v>13.6350407326293</v>
+        <v>0.9999999999825379</v>
       </c>
       <c r="F31" t="n">
-        <v>0.9999999999825379</v>
-      </c>
-      <c r="G31" t="n">
         <v>3.444602467234266e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>B-56</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>200</v>
+      </c>
+      <c r="C32" t="n">
+        <v>20</v>
+      </c>
+      <c r="D32" t="n">
+        <v>13.65917743361162</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.9999999999891415</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2.706368330701313e-05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>B-179</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>200</v>
+      </c>
+      <c r="C33" t="n">
+        <v>20</v>
+      </c>
+      <c r="D33" t="n">
+        <v>13.50204615984026</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.9999999998795512</v>
+      </c>
+      <c r="F33" t="n">
+        <v>9.190995118008015e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>B-180</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>200</v>
+      </c>
+      <c r="C34" t="n">
+        <v>20</v>
+      </c>
+      <c r="D34" t="n">
+        <v>13.49738203688239</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.9999999998625284</v>
+      </c>
+      <c r="F34" t="n">
+        <v>9.818583264019565e-05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Pm_1</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>200</v>
+      </c>
+      <c r="C35" t="n">
+        <v>20</v>
+      </c>
+      <c r="D35" t="n">
+        <v>13.18960068964967</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.9999999999964125</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.553132611592364e-05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>B-64</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>200</v>
+      </c>
+      <c r="C36" t="n">
+        <v>20</v>
+      </c>
+      <c r="D36" t="n">
+        <v>13.97615737563687</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.9999999999029033</v>
+      </c>
+      <c r="F36" t="n">
+        <v>8.108247201563344e-05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>B-38</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>200</v>
+      </c>
+      <c r="C37" t="n">
+        <v>20</v>
+      </c>
+      <c r="D37" t="n">
+        <v>20.20308950931859</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.9999999997344743</v>
+      </c>
+      <c r="F37" t="n">
+        <v>9.888641198894909e-05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>B-21</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>200</v>
+      </c>
+      <c r="C38" t="n">
+        <v>500</v>
+      </c>
+      <c r="D38" t="n">
+        <v>31.82315934299833</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.9999999999671176</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2.169281183303591e-05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>B-30</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>200</v>
+      </c>
+      <c r="C39" t="n">
+        <v>500</v>
+      </c>
+      <c r="D39" t="n">
+        <v>31.4903696039259</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.9999999999776172</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.786205246302725e-05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>B-39</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>200</v>
+      </c>
+      <c r="C40" t="n">
+        <v>500</v>
+      </c>
+      <c r="D40" t="n">
+        <v>33.22439110305697</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9999999999635034</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2.134185682007395e-05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>B-48</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>200</v>
+      </c>
+      <c r="C41" t="n">
+        <v>500</v>
+      </c>
+      <c r="D41" t="n">
+        <v>31.44993653738167</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.9999999999786442</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1.672898120417109e-05</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>B-63</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>200</v>
+      </c>
+      <c r="C42" t="n">
+        <v>500</v>
+      </c>
+      <c r="D42" t="n">
+        <v>32.4854722491454</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.9999999999999915</v>
+      </c>
+      <c r="F42" t="n">
+        <v>3.259760537672952e-07</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>B-13</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>200</v>
+      </c>
+      <c r="C43" t="n">
+        <v>500</v>
+      </c>
+      <c r="D43" t="n">
+        <v>31.22200522379606</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.9999999999780108</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1.688105174858925e-05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>B-56</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>200</v>
+      </c>
+      <c r="C44" t="n">
+        <v>500</v>
+      </c>
+      <c r="D44" t="n">
+        <v>31.27955742486905</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.9999999999780357</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.68085614650516e-05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>B-179</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>200</v>
+      </c>
+      <c r="C45" t="n">
+        <v>500</v>
+      </c>
+      <c r="D45" t="n">
+        <v>30.94136303039614</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.9999999999819403</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.553087633237962e-05</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>B-180</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>200</v>
+      </c>
+      <c r="C46" t="n">
+        <v>500</v>
+      </c>
+      <c r="D46" t="n">
+        <v>30.92209530573327</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.9999999999832121</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1.497754728395754e-05</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>B-38</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>200</v>
+      </c>
+      <c r="C47" t="n">
+        <v>500</v>
+      </c>
+      <c r="D47" t="n">
+        <v>33.25127371712366</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.9999999999813809</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3.182136556752954e-05</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>B-64</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>200</v>
+      </c>
+      <c r="C48" t="n">
+        <v>500</v>
+      </c>
+      <c r="D48" t="n">
+        <v>31.82004119965124</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.9997823786276323</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.1075126786957749</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Pm_1</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>200</v>
+      </c>
+      <c r="C49" t="n">
+        <v>500</v>
+      </c>
+      <c r="D49" t="n">
+        <v>30.00673489121017</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.9999999999946135</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1.673171504203359e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>